<commit_message>
Finished demo2. Fixed both known bugs. QueueAnimation works (Probably).
</commit_message>
<xml_diff>
--- a/options-phase.xlsx
+++ b/options-phase.xlsx
@@ -54,9 +54,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>[CodePen]()</t>
-  </si>
-  <si>
     <t>queueAnimation</t>
   </si>
   <si>
@@ -102,10 +99,13 @@
     <t>Callback function that runs once the animation starts</t>
   </si>
   <si>
-    <t>Callback function that runs once the animation has finished</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Callback function that runs once the animation has fully completed. Does not run if animation is replaced by another `goPhase()` call.</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/JexvLW)</t>
   </si>
 </sst>
 </file>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,33 +479,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -522,10 +522,10 @@
         <v>0.8</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -539,10 +539,10 @@
         <v>1.3</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,21 +550,21 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -573,27 +573,27 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>